<commit_message>
Cambios en final_results + LaTeX
</commit_message>
<xml_diff>
--- a/final_results/1/counting.xlsx
+++ b/final_results/1/counting.xlsx
@@ -1,37 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorge/Desktop/tfg-ci/Pruebas_finales/1/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A048A5E1-5C7C-F84E-9ECD-0349AABDFA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="32360" yWindow="1580" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Encontrados_GitHub</t>
+  </si>
+  <si>
+    <t>Encontrados_GitLab</t>
+  </si>
+  <si>
+    <t>jenkins</t>
+  </si>
+  <si>
+    <t>travis</t>
+  </si>
+  <si>
+    <t>circle ci</t>
+  </si>
+  <si>
+    <t>github actions</t>
+  </si>
+  <si>
+    <t>azure pipelines</t>
+  </si>
+  <si>
+    <t>bamboo</t>
+  </si>
+  <si>
+    <t>concourse</t>
+  </si>
+  <si>
+    <t>gitlab ci</t>
+  </si>
+  <si>
+    <t>codeship</t>
+  </si>
+  <si>
+    <t>teamcity</t>
+  </si>
+  <si>
+    <t>bazel</t>
+  </si>
+  <si>
+    <t>semaphore ci</t>
+  </si>
+  <si>
+    <t>appveyor</t>
+  </si>
+  <si>
+    <t>totales</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +105,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,210 +429,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Encontrados_GitHub</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Encontrados_GitLab</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>jenkins</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>7</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>travis</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>129</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>37</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>circle ci</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>62</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>github actions</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>450</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>19</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>azure pipelines</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>bamboo</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>concourse</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>4</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>gitlab ci</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>488</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>codeship</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>teamcity</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>bazel</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>1</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>semaphore ci</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>appveyor</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>totales</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
         <v>568</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>502</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Histogramas en ficheros excel + LaTeX
</commit_message>
<xml_diff>
--- a/final_results/1/counting.xlsx
+++ b/final_results/1/counting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorge/Desktop/tfg-ci/Pruebas_finales/1/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A048A5E1-5C7C-F84E-9ECD-0349AABDFA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F25E62-E77B-FA47-9907-1F216D2A5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32360" yWindow="1580" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,6 +145,2171 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Encontrados_GitHub</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>jenkins</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>travis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>circle ci</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>github actions</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>azure pipelines</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>bamboo</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>concourse</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>gitlab ci</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>codeship</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>teamcity</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>bazel</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>semaphore ci</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>appveyor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-892C-0341-9B91-2385C2425BA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Encontrados_GitLab</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>jenkins</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>travis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>circle ci</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>github actions</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>azure pipelines</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>bamboo</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>concourse</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>gitlab ci</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>codeship</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>teamcity</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>bazel</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>semaphore ci</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>appveyor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-892C-0341-9B91-2385C2425BA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="1885228703"/>
+        <c:axId val="1884876927"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1885228703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1884876927"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1884876927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1885228703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Encontrados_GitHub</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>totales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>568</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AC71-FF43-8C4D-79FC34AD5DA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Encontrados_GitLab</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>totales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AC71-FF43-8C4D-79FC34AD5DA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="1837594975"/>
+        <c:axId val="1833365023"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1837594975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1833365023"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1833365023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1837594975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A66A9B-C0B2-D74A-A2AF-ECF9D8388341}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76F6FE0A-214D-CA46-AA9F-D6C5B3378DFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -432,7 +2597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -605,5 +2772,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>